<commit_message>
Finalized analysis and text.
</commit_message>
<xml_diff>
--- a/Challenge Datasets/results.xlsx
+++ b/Challenge Datasets/results.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anders/OneDrive - Heinrich-Heine-Universitat Dusseldorf/kinSoftChallenge2019/Challenge Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniduesseldorf-my.sharepoint.com/personal/anders_barth_office365_hhu_de/Documents/kinSoftChallenge2019/Challenge Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="8_{7B7E97BA-856B-6741-94A6-921E2B787EBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{412A0A05-DBBC-504B-BEBC-448D0CD60743}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="8_{7B7E97BA-856B-6741-94A6-921E2B787EBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C218BFBF-97B9-B04D-884C-1867CA125B8E}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="460" windowWidth="38400" windowHeight="19760" activeTab="2" xr2:uid="{5B49C4A4-8F53-5748-8807-C34DBD0EA146}"/>
+    <workbookView xWindow="19740" yWindow="540" windowWidth="38400" windowHeight="20360" activeTab="4" xr2:uid="{5B49C4A4-8F53-5748-8807-C34DBD0EA146}"/>
   </bookViews>
   <sheets>
-    <sheet name="sim_level1_final_publish" sheetId="1" r:id="rId1"/>
-    <sheet name="sim_level2_final_publish" sheetId="2" r:id="rId2"/>
-    <sheet name="sim_level3_final_publish" sheetId="3" r:id="rId3"/>
+    <sheet name="Summary" sheetId="4" r:id="rId1"/>
+    <sheet name="sim_level1_final_publish" sheetId="1" r:id="rId2"/>
+    <sheet name="sim_level2_final_publish" sheetId="2" r:id="rId3"/>
+    <sheet name="sim_level3_final_publish" sheetId="3" r:id="rId4"/>
+    <sheet name="Test dataset" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
   <si>
     <t>red. Chi2</t>
   </si>
@@ -129,6 +131,156 @@
   </si>
   <si>
     <t>mcmc_average</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>Amp</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>0.72 ± 0.09 (40.2%)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0.286 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.420 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.24 ± 0.08 (59.8%)</t>
+  </si>
+  <si>
+    <t>0.18 ± 0.10 (66.0%)</t>
+  </si>
+  <si>
+    <t>0.73 ± 0.10 (34%)</t>
+  </si>
+  <si>
+    <t>0.64 ± 0.09</t>
+  </si>
+  <si>
+    <t>5 ± 2</t>
+  </si>
+  <si>
+    <t>20 ± 11</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>fFCS</t>
+  </si>
+  <si>
+    <t>FRET-FCS</t>
+  </si>
+  <si>
+    <t>Descr. 3 exp</t>
+  </si>
+  <si>
+    <t>Descr. 2 exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.80+ 0.07 </t>
+  </si>
+  <si>
+    <t>0.425 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.091 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.284 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.560 ± 0.005</t>
+  </si>
+  <si>
+    <t>0.249 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.173 ± 0.003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.280 ± 0.003 </t>
+  </si>
+  <si>
+    <t>0.90 ± 0.09 (40.9%)</t>
+  </si>
+  <si>
+    <t>0.10 ± 0.09 (28.9%)</t>
+  </si>
+  <si>
+    <t>0.53 ± 0.08 (30.2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.7± 0.6 </t>
+  </si>
+  <si>
+    <t>red, chi2</t>
+  </si>
+  <si>
+    <t>fFCS descriptive model 4 exp</t>
+  </si>
+  <si>
+    <t>chi2red</t>
+  </si>
+  <si>
+    <t>Truth</t>
+  </si>
+  <si>
+    <t>0.990 ± 0.004</t>
+  </si>
+  <si>
+    <t>0.647 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.921 ± 0.004</t>
+  </si>
+  <si>
+    <t>0.64 ± 0.005</t>
+  </si>
+  <si>
+    <t>0.240 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.152 ± 0.002</t>
+  </si>
+  <si>
+    <t>0.0022 ± 0.0006</t>
+  </si>
+  <si>
+    <t>0.468 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.347 ± 0.003</t>
+  </si>
+  <si>
+    <t>0.087 ± 0.002</t>
+  </si>
+  <si>
+    <t>average trace length: 50</t>
+  </si>
+  <si>
+    <t>1 ± 1</t>
+  </si>
+  <si>
+    <t>1.3 ± 0.6</t>
+  </si>
+  <si>
+    <t>8 ± 2</t>
   </si>
 </sst>
 </file>
@@ -177,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -186,6 +338,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,11 +655,280 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639523E7-B865-0646-A89C-DDA4B0535127}">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>71.38</v>
+      </c>
+      <c r="I7">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8">
+        <v>68.89</v>
+      </c>
+      <c r="I8">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15">
+        <v>5.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA03A5F4-1E0C-3845-9851-AB3D4E339D33}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="134" zoomScaleNormal="218" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,12 +1034,29 @@
         <v>2.6061044310101201E-3</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.24</v>
+        <v>0.242196489067312</v>
+      </c>
+      <c r="C14">
+        <v>7.8398120385723996E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.59812039502090897</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -622,7 +1064,13 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.72</v>
+        <v>0.72267182647871098</v>
+      </c>
+      <c r="C15">
+        <v>8.4742732122474199E-2</v>
+      </c>
+      <c r="D15">
+        <v>0.40187960497909098</v>
       </c>
     </row>
   </sheetData>
@@ -630,12 +1078,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46D7295-1C75-9743-8360-35A1826A104B}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="227" zoomScaleNormal="227" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -810,17 +1258,70 @@
         <v>2.5099945396160998E-3</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.89866994258780497</v>
+      </c>
+      <c r="C16">
+        <v>9.2890480847970205E-2</v>
+      </c>
+      <c r="D16">
+        <v>0.40907405532859198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>9.9503403520699807E-2</v>
+      </c>
+      <c r="C17">
+        <v>9.1170426765926293E-2</v>
+      </c>
+      <c r="D17">
+        <v>0.289383471990105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>0.52723373848231703</v>
+      </c>
+      <c r="C18">
+        <v>7.4483934693140602E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.30154247268130302</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051B6D58-9AC5-6443-881B-722F0CAFCC7C}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1032,7 +1533,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D18">
         <v>0.03</v>
@@ -1102,6 +1603,310 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>0.18264855361064</v>
+      </c>
+      <c r="C27">
+        <v>9.7494309758002898E-2</v>
+      </c>
+      <c r="D27">
+        <v>0.65969636789877195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>0.72501897896183398</v>
+      </c>
+      <c r="C28">
+        <v>9.4881406006735905E-2</v>
+      </c>
+      <c r="D28">
+        <v>0.33541971117640001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29">
+        <v>0.38259521130849999</v>
+      </c>
+      <c r="C29">
+        <v>0.77002598010635803</v>
+      </c>
+      <c r="D29">
+        <v>4.8839209248285496E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED4BE4E-F1E2-9A40-93D6-73324C65215D}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5">
+        <v>0.32</v>
+      </c>
+      <c r="D5">
+        <v>0.11</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.06</v>
+      </c>
+      <c r="G5">
+        <v>0.39</v>
+      </c>
+      <c r="H5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8">
+        <v>0.78</v>
+      </c>
+      <c r="D8">
+        <v>5.31</v>
+      </c>
+      <c r="E8">
+        <v>23.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9">
+        <v>169.72</v>
+      </c>
+      <c r="I9">
+        <v>0.36</v>
+      </c>
+      <c r="J9" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed wrong time windows for challenge 1 and 3.
</commit_message>
<xml_diff>
--- a/Challenge Datasets/results.xlsx
+++ b/Challenge Datasets/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniduesseldorf-my.sharepoint.com/personal/anders_barth_office365_hhu_de/Documents/kinSoftChallenge2019/Challenge Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniduesseldorf-my.sharepoint.com/personal/anders_barth_office365_hhu_de/Documents/kinSoftChallenge/repo/Challenge Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="441" documentId="8_{7B7E97BA-856B-6741-94A6-921E2B787EBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C218BFBF-97B9-B04D-884C-1867CA125B8E}"/>
+  <xr:revisionPtr revIDLastSave="555" documentId="8_{7B7E97BA-856B-6741-94A6-921E2B787EBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C9B7164D-4EDD-8348-84DD-006C0E0FD9D0}"/>
   <bookViews>
-    <workbookView xWindow="19740" yWindow="540" windowWidth="38400" windowHeight="20360" activeTab="4" xr2:uid="{5B49C4A4-8F53-5748-8807-C34DBD0EA146}"/>
+    <workbookView xWindow="6700" yWindow="680" windowWidth="33600" windowHeight="19720" xr2:uid="{5B49C4A4-8F53-5748-8807-C34DBD0EA146}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
   <si>
     <t>red. Chi2</t>
   </si>
@@ -112,12 +112,6 @@
     <t>tau4</t>
   </si>
   <si>
-    <t>insufficient sampling because nlparci estimate is too high for tau1</t>
-  </si>
-  <si>
-    <t>bascially, it does not yield anything that makes sense</t>
-  </si>
-  <si>
     <t>lower</t>
   </si>
   <si>
@@ -154,12 +148,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>0.286 ± 0.003</t>
-  </si>
-  <si>
-    <t>0.420 ± 0.003</t>
-  </si>
-  <si>
     <t>0.24 ± 0.08 (59.8%)</t>
   </si>
   <si>
@@ -169,15 +157,6 @@
     <t>0.73 ± 0.10 (34%)</t>
   </si>
   <si>
-    <t>0.64 ± 0.09</t>
-  </si>
-  <si>
-    <t>5 ± 2</t>
-  </si>
-  <si>
-    <t>20 ± 11</t>
-  </si>
-  <si>
     <t>Method</t>
   </si>
   <si>
@@ -193,12 +172,6 @@
     <t>Descr. 2 exp</t>
   </si>
   <si>
-    <t xml:space="preserve">0.80+ 0.07 </t>
-  </si>
-  <si>
-    <t>0.425 ± 0.003</t>
-  </si>
-  <si>
     <t>0.091 ± 0.003</t>
   </si>
   <si>
@@ -226,9 +199,6 @@
     <t>0.53 ± 0.08 (30.2%)</t>
   </si>
   <si>
-    <t xml:space="preserve">11.7± 0.6 </t>
-  </si>
-  <si>
     <t>red, chi2</t>
   </si>
   <si>
@@ -274,13 +244,49 @@
     <t>average trace length: 50</t>
   </si>
   <si>
-    <t>1 ± 1</t>
-  </si>
-  <si>
-    <t>1.3 ± 0.6</t>
-  </si>
-  <si>
-    <t>8 ± 2</t>
+    <t>2.6 ± 1.2</t>
+  </si>
+  <si>
+    <t>2 ± 2</t>
+  </si>
+  <si>
+    <t>16 ± 4</t>
+  </si>
+  <si>
+    <t>lb mcmc</t>
+  </si>
+  <si>
+    <t>ub mcmc</t>
+  </si>
+  <si>
+    <t>mean mcmc</t>
+  </si>
+  <si>
+    <t>0.143 ± 0.002</t>
+  </si>
+  <si>
+    <t>0.210± 0.002</t>
+  </si>
+  <si>
+    <t>0.212 ± 0.002</t>
+  </si>
+  <si>
+    <t>0.143 ± 0.002</t>
+  </si>
+  <si>
+    <t>1.6 ± 0.2</t>
+  </si>
+  <si>
+    <t>23.4 ± 1.2</t>
+  </si>
+  <si>
+    <t>1.3 ± 0.2</t>
+  </si>
+  <si>
+    <t>10.6 ± 4.3</t>
+  </si>
+  <si>
+    <t>40 ± 16</t>
   </si>
 </sst>
 </file>
@@ -658,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639523E7-B865-0646-A89C-DDA4B0535127}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,10 +680,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -700,7 +706,7 @@
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -708,25 +714,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I3">
         <v>1.07</v>
@@ -737,25 +743,25 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I4">
         <v>0.998</v>
@@ -766,25 +772,25 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" t="s">
-        <v>57</v>
-      </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I5">
         <v>1.83</v>
@@ -812,16 +818,16 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H7">
         <v>71.38</v>
@@ -832,16 +838,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="H8">
         <v>68.89</v>
@@ -852,7 +858,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -861,10 +867,10 @@
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -872,13 +878,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13">
         <v>3.7</v>
@@ -889,13 +895,13 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E14">
         <v>7.1</v>
@@ -906,13 +912,13 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15">
         <v>5.2</v>
@@ -927,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA03A5F4-1E0C-3845-9851-AB3D4E339D33}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="218" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A3" zoomScale="134" zoomScaleNormal="218" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -962,13 +968,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.28582985263028099</v>
+        <v>0.14291492631514049</v>
       </c>
       <c r="C4">
-        <v>3.62019486156812E-3</v>
+        <v>1.81009743078406E-3</v>
       </c>
       <c r="D4">
-        <v>2.5953827612343701E-3</v>
+        <v>1.297691380617185E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -976,13 +982,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.42475028340090798</v>
+        <v>0.21237514170045399</v>
       </c>
       <c r="C5">
-        <v>4.2640951133007801E-3</v>
+        <v>2.13204755665039E-3</v>
       </c>
       <c r="D5">
-        <v>2.97398650147005E-3</v>
+        <v>1.486993250735025E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1011,13 +1017,13 @@
         <v>3</v>
       </c>
       <c r="B11">
-        <v>0.286240042661982</v>
+        <v>0.143120021330991</v>
       </c>
       <c r="C11">
-        <v>4.3674289091159002E-3</v>
+        <v>2.1837144545579501E-3</v>
       </c>
       <c r="D11">
-        <v>2.87213860234672E-3</v>
+        <v>1.43606930117336E-3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1025,24 +1031,24 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <v>0.41998946610830301</v>
+        <v>0.20999473305415151</v>
       </c>
       <c r="C12">
-        <v>3.7366296768155398E-3</v>
+        <v>1.8683148384077699E-3</v>
       </c>
       <c r="D12">
-        <v>2.6061044310101201E-3</v>
+        <v>1.3030522155050601E-3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
         <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1260,13 +1266,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
         <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1299,7 +1305,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>0.52723373848231703</v>
@@ -1321,7 +1327,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,13 +1370,13 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>0.79294066604764102</v>
+        <v>1.585881332095282</v>
       </c>
       <c r="C4">
-        <v>3.1361933282181599E-2</v>
+        <v>6.2723866564363198E-2</v>
       </c>
       <c r="D4">
-        <v>6.8899868250240803E-2</v>
+        <v>0.13779973650048161</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1378,13 +1384,13 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>11.7056823269963</v>
+        <v>23.411364653992599</v>
       </c>
       <c r="C5">
-        <v>0.28021941337436501</v>
+        <v>0.56043882674873002</v>
       </c>
       <c r="D5">
-        <v>0.60427081253402704</v>
+        <v>1.2085416250680541</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1417,7 +1423,7 @@
         <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1428,16 +1434,16 @@
         <v>5</v>
       </c>
       <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
         <v>27</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" t="s">
         <v>29</v>
-      </c>
-      <c r="I11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1445,23 +1451,26 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.63484029724347502</v>
+        <v>1.26968059448695</v>
       </c>
       <c r="C12" s="4">
-        <v>2.2840351711394501E-2</v>
+        <v>4.5681540878748303E-2</v>
       </c>
       <c r="D12">
-        <v>8.9231440827607394E-2</v>
+        <v>0.181852919555957</v>
       </c>
       <c r="G12">
-        <v>0.56999999999999995</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="H12">
-        <v>0.74</v>
+        <v>1.47</v>
       </c>
       <c r="I12">
         <f>(H12-G12)/2</f>
-        <v>8.500000000000002E-2</v>
+        <v>0.17999999999999994</v>
+      </c>
+      <c r="J12">
+        <v>1.29</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1469,23 +1478,26 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>5.2791472025405799</v>
+        <v>10.55829440508116</v>
       </c>
       <c r="C13">
-        <v>0.60896580187634997</v>
+        <v>1.2179146348889001</v>
       </c>
       <c r="D13">
-        <v>2.24018420143112</v>
+        <v>4.3207897432775999</v>
       </c>
       <c r="G13">
-        <v>3.76</v>
+        <v>6.55</v>
       </c>
       <c r="H13">
-        <v>8.19</v>
+        <v>15.2</v>
       </c>
       <c r="I13">
         <f t="shared" ref="I13:I14" si="0">(H13-G13)/2</f>
-        <v>2.2149999999999999</v>
+        <v>4.3249999999999993</v>
+      </c>
+      <c r="J13">
+        <v>10.84</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1493,26 +1505,26 @@
         <v>23</v>
       </c>
       <c r="B14">
-        <v>19.8346306529317</v>
+        <v>39.669261305863401</v>
       </c>
       <c r="C14">
-        <v>2.0293037051979099</v>
+        <v>4.05814711645034</v>
       </c>
       <c r="D14">
-        <v>10.741315941373999</v>
+        <v>16.165882872713102</v>
       </c>
       <c r="G14">
-        <v>15.47</v>
+        <v>29.88</v>
       </c>
       <c r="H14">
-        <v>39.073</v>
+        <v>62.21</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>11.801500000000001</v>
+        <v>16.164999999999999</v>
       </c>
       <c r="J14">
-        <v>23.125399999999999</v>
+        <v>40.869999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1520,7 +1532,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1531,9 +1543,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D18">
         <v>0.03</v>
@@ -1542,81 +1554,132 @@
         <v>91.19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20">
-        <v>8.7840619378341707E-3</v>
-      </c>
-      <c r="C20" s="5">
-        <v>319.376796513334</v>
-      </c>
-      <c r="D20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.2912498917451201</v>
+      </c>
+      <c r="C20" s="4">
+        <v>7.3697916892334903E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.191896573454437</v>
+      </c>
+      <c r="E20">
+        <v>1.1176422111169899</v>
+      </c>
+      <c r="F20">
+        <v>1.5014353580258699</v>
+      </c>
+      <c r="G20">
+        <v>1.2886533120308501</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21">
-        <v>0.63470453176363995</v>
-      </c>
-      <c r="C21">
-        <v>3.3001486166105203E-2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8.2196952521770594</v>
+      </c>
+      <c r="C21" s="5">
+        <v>14.198381069147199</v>
+      </c>
+      <c r="D21">
+        <v>4.9159190674142499</v>
+      </c>
+      <c r="E21">
+        <v>6.2860209364926396</v>
+      </c>
+      <c r="F21">
+        <v>16.117859071321099</v>
+      </c>
+      <c r="G21">
+        <v>10.3547555461719</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22">
-        <v>5.2646801888924299</v>
-      </c>
-      <c r="C22">
-        <v>0.64001634695403398</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11.1813615404667</v>
+      </c>
+      <c r="C22" s="5">
+        <v>11.513218455953799</v>
+      </c>
+      <c r="D22">
+        <v>5.25752322026585</v>
+      </c>
+      <c r="E22">
+        <v>6.2294893852969802</v>
+      </c>
+      <c r="F22">
+        <v>16.744535825828699</v>
+      </c>
+      <c r="G22">
+        <v>10.5219809236452</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
-        <v>19.7985757346339</v>
+        <v>39.305473426660598</v>
       </c>
       <c r="C23">
-        <v>2.0604021942256798</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8.6387524019556903</v>
+      </c>
+      <c r="D23">
+        <v>12.074579660976299</v>
+      </c>
+      <c r="E23">
+        <v>30.035411026022999</v>
+      </c>
+      <c r="F23">
+        <v>54.184570347975601</v>
+      </c>
+      <c r="G23">
+        <v>37.220201467046003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
         <v>33</v>
       </c>
-      <c r="D26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1630,7 +1693,7 @@
         <v>0.65969636789877195</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1644,9 +1707,9 @@
         <v>0.33541971117640001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>0.38259521130849999</v>
@@ -1667,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED4BE4E-F1E2-9A40-93D6-73324C65215D}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1681,10 +1744,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1705,7 +1768,7 @@
         <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1713,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1723,16 +1786,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I2" s="6"/>
     </row>
@@ -1741,25 +1804,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I3">
         <v>1.75</v>
@@ -1770,25 +1833,25 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I4">
         <v>0.85</v>
@@ -1799,7 +1862,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C5">
         <v>0.32</v>
@@ -1825,25 +1888,25 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="I6">
         <v>1.25</v>
@@ -1871,7 +1934,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C8">
         <v>0.78</v>
@@ -1888,16 +1951,16 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H9">
         <v>169.72</v>
@@ -1906,7 +1969,7 @@
         <v>0.36</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>